<commit_message>
updated test names got getDistances
for consistency with matrix
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_getTruckDistances2.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_getTruckDistances2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cescadelacruz/Documents/GitHub/SUM23-SFT221-NAA-4/Documents/Testing/TestsDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7277CCAD-C4A1-9A4E-ADA5-17A1177B6820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B14FD95-433E-B142-BBB7-43A59DBCF45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>SFT 221</t>
   </si>
@@ -343,6 +343,9 @@
 To calculate the distances of each truck, the function first retrieves the closest point of each truck by calling getClosestPoint(). Then it calculates the distance from the destination of each truck by calling distance(), with the values returned from getClosestPoint() and “destination” as arguments.
 Afterward, it populates the “arr” array with the trucks’ distances and corresponding colour codes and sorts the distances in the array.
 The purpose of the test is to ensure the function calculates and populates the “arr” array correctly, by verifying every index is filled correctly with the truck’s distances and colour codes.</t>
+  </si>
+  <si>
+    <t>FUNCTION: getTruckDistances2</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1058,7 +1061,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1344,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1665,15 +1668,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008641478389A1824A98F5C5E0B6162E5F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ef4b42a3ed9448361827c423e89ef89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81b064ac-ebcb-49a1-93f6-e61f75bebfa7" xmlns:ns3="717d1b07-b5a1-4bb5-9d40-3a9b6c764643" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bb8b9f62ca6562dff4b6b6c0721aa08" ns2:_="" ns3:_="">
     <xsd:import namespace="81b064ac-ebcb-49a1-93f6-e61f75bebfa7"/>
@@ -1844,6 +1838,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
   <ds:schemaRefs>
@@ -1862,14 +1865,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A5AAF0-BBBC-48E3-AADB-8E4922D37D7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1886,4 +1881,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>